<commit_message>
add ABCD labels to histogram chart
</commit_message>
<xml_diff>
--- a/Data/DivingElephantSeals.xlsx
+++ b/Data/DivingElephantSeals.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\drp36\OneDrive - BYU-Idaho 1\221\Course_Files\BYUI_M221_Book\Data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="420" windowWidth="19440" windowHeight="9495"/>
   </bookViews>
@@ -11,12 +16,12 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="125725" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="37">
   <si>
     <t>Chick</t>
   </si>
@@ -79,9 +84,6 @@
   </si>
   <si>
     <t>Arterial (femoral)</t>
-  </si>
-  <si>
-    <t>65..8</t>
   </si>
   <si>
     <t>Representative Temperature</t>
@@ -135,8 +137,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -197,6 +199,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -243,7 +253,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -275,9 +285,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -309,6 +320,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -484,14 +496,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.28515625" bestFit="1" customWidth="1"/>
@@ -502,9 +514,9 @@
     <col min="14" max="14" width="27.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="1" customFormat="1">
+    <row r="1" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>14</v>
@@ -519,37 +531,37 @@
         <v>16</v>
       </c>
       <c r="F1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="I1" s="2" t="s">
-        <v>35</v>
-      </c>
       <c r="J1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="K1" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="N1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="O1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="N1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15">
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -593,10 +605,10 @@
         <v>36.700000000000003</v>
       </c>
       <c r="O2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -640,10 +652,10 @@
         <v>37.19</v>
       </c>
       <c r="O3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -687,10 +699,10 @@
         <v>37.85</v>
       </c>
       <c r="O4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -734,10 +746,10 @@
         <v>37.909999999999997</v>
       </c>
       <c r="O5" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -781,10 +793,10 @@
         <v>37.25</v>
       </c>
       <c r="O6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -828,7 +840,7 @@
         <v>38.979999999999997</v>
       </c>
     </row>
-    <row r="8" spans="1:15">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -872,7 +884,7 @@
         <v>38.159999999999997</v>
       </c>
     </row>
-    <row r="9" spans="1:15">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -900,8 +912,8 @@
       <c r="I9">
         <v>11.7</v>
       </c>
-      <c r="J9" t="s">
-        <v>21</v>
+      <c r="J9">
+        <v>65.8</v>
       </c>
       <c r="K9">
         <v>28.4</v>
@@ -916,7 +928,7 @@
         <v>39.32</v>
       </c>
     </row>
-    <row r="10" spans="1:15">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -960,7 +972,7 @@
         <v>39.700000000000003</v>
       </c>
     </row>
-    <row r="11" spans="1:15">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -1004,7 +1016,7 @@
         <v>39.71</v>
       </c>
     </row>
-    <row r="12" spans="1:15">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -1048,7 +1060,7 @@
         <v>35.770000000000003</v>
       </c>
     </row>
-    <row r="13" spans="1:15">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -1092,7 +1104,7 @@
         <v>38.47</v>
       </c>
     </row>
-    <row r="14" spans="1:15">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -1142,24 +1154,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>